<commit_message>
Readme correction and ExcelParser bug fixed
</commit_message>
<xml_diff>
--- a/demoExcelSpec.xlsx
+++ b/demoExcelSpec.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Assemblies Info" sheetId="1" r:id="rId1"/>
-    <sheet name="Assemblies Specifications" sheetId="2" r:id="rId2"/>
+    <sheet name="Assembly Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Assembly Specification" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -26,15 +26,9 @@
     <t>Grapher</t>
   </si>
   <si>
-    <t>Model engine</t>
-  </si>
-  <si>
     <t>MSAGL</t>
   </si>
   <si>
-    <t>DependenciesModel</t>
-  </si>
-  <si>
     <t>Microsoft.Msagl*</t>
   </si>
   <si>
@@ -47,9 +41,6 @@
     <t>Newtonsoft.Json</t>
   </si>
   <si>
-    <t>ModelApplications</t>
-  </si>
-  <si>
     <t>Other external sources</t>
   </si>
   <si>
@@ -92,7 +83,16 @@
     <t>Signed</t>
   </si>
   <si>
-    <t>DotNETAssembliesGrapher</t>
+    <t>DotNETAssemblyGrapher</t>
+  </si>
+  <si>
+    <t>DotNETAssemblyGrapher.Model</t>
+  </si>
+  <si>
+    <t>DotNETAssemblyGrapher.Application</t>
+  </si>
+  <si>
+    <t>External sources</t>
   </si>
 </sst>
 </file>
@@ -123,12 +123,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -136,6 +130,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,36 +175,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -510,20 +505,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -533,60 +528,61 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="13" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="9" t="s">
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A2:A5"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -596,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -608,112 +604,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>23</v>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="11"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>12</v>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="11"/>
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11" t="s">
-        <v>12</v>
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>